<commit_message>
Compare_fdm3t case Bruggeman 220-03 also ok. Verified with Modflow, fdm3t and ttim.
</commit_message>
<xml_diff>
--- a/Projects/Compare_fdm3t/cases/Brug223_02/Brug223_02.xlsx
+++ b/Projects/Compare_fdm3t/cases/Brug223_02/Brug223_02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/Compare_fdm3t/cases/Brug223_02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF26EEF2-B232-5142-AFA8-BC9FBE78BDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F6D16C-8531-4740-8B1E-238D9DEBE92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9820" yWindow="-24220" windowWidth="28180" windowHeight="16980" tabRatio="751" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13700" yWindow="-24240" windowWidth="28180" windowHeight="16980" tabRatio="751" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>

</xml_diff>